<commit_message>
feat(exercise-to-day-and-fix): adiciona exercicio completos.
</commit_message>
<xml_diff>
--- a/back-end/Block-21-SQL-Functions,-JOINs-and-Normalization/day-03-Transforming-ideas-into-a-database-model/exercise-to-day/exercise-3.xlsx
+++ b/back-end/Block-21-SQL-Functions,-JOINs-and-Normalization/day-03-Transforming-ideas-into-a-database-model/exercise-to-day/exercise-3.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
   <si>
     <t xml:space="preserve">TABELA DESNORMALIZADA</t>
   </si>
@@ -92,10 +92,61 @@
     <t xml:space="preserve">nome</t>
   </si>
   <si>
+    <t xml:space="preserve">liga_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">universo_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">criador_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">LIGA</t>
   </si>
   <si>
-    <t xml:space="preserve">liga_id</t>
+    <t xml:space="preserve">X-men</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Justice Legue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNIVERSO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MARVEL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRIADOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sobre_nome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">idade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gardner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Len</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wein</t>
   </si>
 </sst>
 </file>
@@ -420,8 +471,8 @@
   </sheetPr>
   <dimension ref="F1:K12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="1" sqref="B14:D33 F11"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -575,15 +626,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14:D33"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.58"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -598,6 +652,15 @@
       <c r="B3" s="17" t="s">
         <v>22</v>
       </c>
+      <c r="C3" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="17" t="n">
@@ -606,6 +669,15 @@
       <c r="B4" s="17" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="17" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="n">
@@ -613,6 +685,15 @@
       </c>
       <c r="B5" s="17" t="s">
         <v>11</v>
+      </c>
+      <c r="C5" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -622,6 +703,15 @@
       <c r="B6" s="17" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D6" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="17" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="17" t="n">
@@ -630,15 +720,24 @@
       <c r="B7" s="17" t="s">
         <v>18</v>
       </c>
+      <c r="C7" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="17" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>3</v>
@@ -648,19 +747,129 @@
       <c r="A14" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B14" s="17"/>
+      <c r="B14" s="17" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B16" s="17"/>
+      <c r="B16" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="17" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30" s="17" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="17" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="17" t="n">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>